<commit_message>
- renamed res and cap to match the original Circuitmaker  design - fixed BOM file according to changes
</commit_message>
<xml_diff>
--- a/H1AR20/Released/BOM/H1AR20.xlsx
+++ b/H1AR20/Released/BOM/H1AR20.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Hexabitz\Hardware\H1AR2x-Hardware\H1AR20\Released\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -127,9 +127,6 @@
     <t>10.0K</t>
   </si>
   <si>
-    <t>R2</t>
-  </si>
-  <si>
     <t>CAP CER  10% X7R 0603</t>
   </si>
   <si>
@@ -224,12 +221,6 @@
   </si>
   <si>
     <t>IC MCU 32BIT 128KB FLASH 48QFPN</t>
-  </si>
-  <si>
-    <t>R4</t>
-  </si>
-  <si>
-    <t>C4, C7</t>
   </si>
   <si>
     <t>CRCW060368R0FKEA</t>
@@ -276,9 +267,6 @@
     <t>Cree CLVBA-FKA-CC1F1L1BB7R3R3</t>
   </si>
   <si>
-    <t>C1</t>
-  </si>
-  <si>
     <t>100nF</t>
   </si>
   <si>
@@ -309,9 +297,6 @@
     <t>100uF</t>
   </si>
   <si>
-    <t>C11</t>
-  </si>
-  <si>
     <t>Ceramic Capacitor X5R 1210</t>
   </si>
   <si>
@@ -327,9 +312,6 @@
     <t>47pF</t>
   </si>
   <si>
-    <t>C12, C13</t>
-  </si>
-  <si>
     <t>06035A470JAT2A</t>
   </si>
   <si>
@@ -342,9 +324,6 @@
     <t>±10%</t>
   </si>
   <si>
-    <t>C3, C5, C6, C8, C9, C14, C15, C16</t>
-  </si>
-  <si>
     <t>https://octopart.com/10tpu4r7msi-panasonic-29487748</t>
   </si>
   <si>
@@ -390,30 +369,18 @@
     <t>Connector Unshrouded Header HDR 2 Position 2.54mm Solder Straight Thru-Hole</t>
   </si>
   <si>
-    <t>4.7R</t>
-  </si>
-  <si>
     <t xml:space="preserve"> http://octopart.com/crcw06034k70fkea-vishay-39455708</t>
   </si>
   <si>
-    <t>R3, R5</t>
-  </si>
-  <si>
     <t>27.0R</t>
   </si>
   <si>
-    <t>R6, R7</t>
-  </si>
-  <si>
     <t>CRCW060327R0FKEA</t>
   </si>
   <si>
     <t>https://octopart.com/crcw060327r0fkea-vishay-39833156</t>
   </si>
   <si>
-    <t>R9</t>
-  </si>
-  <si>
     <t>39.0R</t>
   </si>
   <si>
@@ -475,6 +442,39 @@
   </si>
   <si>
     <t>Thick Film Resistors - SMD 0602</t>
+  </si>
+  <si>
+    <t>C1, C6, C7, C8, C9, C11, C12, C15</t>
+  </si>
+  <si>
+    <t>C3, C4</t>
+  </si>
+  <si>
+    <t>C5</t>
+  </si>
+  <si>
+    <t>C16</t>
+  </si>
+  <si>
+    <t>C13, C14</t>
+  </si>
+  <si>
+    <t>R2, R9</t>
+  </si>
+  <si>
+    <t>R3</t>
+  </si>
+  <si>
+    <t>4.7K</t>
+  </si>
+  <si>
+    <t>R4, R5</t>
+  </si>
+  <si>
+    <t>R6</t>
+  </si>
+  <si>
+    <t>R7</t>
   </si>
 </sst>
 </file>
@@ -877,8 +877,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -899,10 +899,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>49</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>50</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>1</v>
@@ -914,7 +914,7 @@
         <v>3</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="H1" s="3" t="s">
         <v>4</v>
@@ -928,25 +928,25 @@
         <v>8</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>85</v>
+        <v>119</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="G2" s="1" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -960,7 +960,7 @@
         <v>15</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>11</v>
@@ -980,25 +980,25 @@
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="E4" s="1" t="s">
+      <c r="F4" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>32</v>
       </c>
       <c r="G4" s="4">
         <v>0.1</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -1006,25 +1006,25 @@
         <v>1</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>89</v>
+        <v>63</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -1032,25 +1032,25 @@
         <v>1</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>24</v>
       </c>
       <c r="G6" s="4">
         <v>0.1</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -1058,25 +1058,25 @@
         <v>1</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="F7" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="G7" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="H7" s="2" t="s">
         <v>67</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -1084,25 +1084,25 @@
         <v>1</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="H8" s="2" t="s">
         <v>73</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -1110,25 +1110,25 @@
         <v>2</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>80</v>
+        <v>123</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -1136,23 +1136,23 @@
         <v>1</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="D10" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="E10" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E10" s="1" t="s">
-        <v>42</v>
-      </c>
       <c r="F10" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G10" s="1"/>
       <c r="H10" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -1160,23 +1160,23 @@
         <v>1</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="G11" s="1"/>
       <c r="H11" s="2" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -1184,23 +1184,23 @@
         <v>2</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="D12" s="1" t="s">
+      <c r="E12" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="F12" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>37</v>
       </c>
       <c r="G12" s="1"/>
       <c r="H12" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -1208,23 +1208,23 @@
         <v>1</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="G13" s="1"/>
       <c r="H13" s="2" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -1232,21 +1232,21 @@
         <v>1</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="E14" s="1"/>
       <c r="F14" s="1" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="G14" s="1"/>
       <c r="H14" s="2" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -1254,25 +1254,25 @@
         <v>1</v>
       </c>
       <c r="B15" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C15" s="1" t="s">
-        <v>27</v>
-      </c>
       <c r="D15" s="1" t="s">
-        <v>129</v>
+        <v>118</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G15" s="4">
         <v>0.01</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -1280,25 +1280,25 @@
         <v>1</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>114</v>
+        <v>103</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>115</v>
+        <v>104</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -1309,7 +1309,7 @@
         <v>9</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>19</v>
+        <v>125</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>10</v>
@@ -1333,22 +1333,22 @@
         <v>18</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>103</v>
+        <v>124</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>112</v>
+        <v>101</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>113</v>
+        <v>102</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -1356,25 +1356,25 @@
         <v>1</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>101</v>
+        <v>126</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>52</v>
+        <v>117</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="G19" s="4">
         <v>0.01</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -1382,25 +1382,25 @@
         <v>2</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>105</v>
+        <v>127</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="G20" s="4">
         <v>0.01</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
@@ -1408,25 +1408,25 @@
         <v>1</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>109</v>
+        <v>98</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>108</v>
+        <v>128</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>110</v>
+        <v>99</v>
       </c>
       <c r="G21" s="4">
         <v>0.05</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>111</v>
+        <v>100</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
@@ -1440,7 +1440,7 @@
         <v>6</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>7</v>
@@ -1458,23 +1458,23 @@
         <v>1</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>118</v>
+        <v>107</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>116</v>
+        <v>105</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>124</v>
+        <v>113</v>
       </c>
       <c r="G23" s="1"/>
       <c r="H23" s="2" t="s">
-        <v>126</v>
+        <v>115</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
@@ -1482,23 +1482,23 @@
         <v>1</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>117</v>
+        <v>106</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="G24" s="1"/>
       <c r="H24" s="2" t="s">
-        <v>125</v>
+        <v>114</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
@@ -1506,23 +1506,23 @@
         <v>1</v>
       </c>
       <c r="B25" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C25" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C25" s="1" t="s">
+      <c r="D25" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="D25" s="1" t="s">
+      <c r="E25" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F25" s="1" t="s">
         <v>46</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>47</v>
       </c>
       <c r="G25" s="1"/>
       <c r="H25" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- PCB is done - Generated all output files
</commit_message>
<xml_diff>
--- a/H1AR20/Released/BOM/H1AR20.xlsx
+++ b/H1AR20/Released/BOM/H1AR20.xlsx
@@ -878,7 +878,7 @@
   <dimension ref="A1:I25"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1458,23 +1458,23 @@
         <v>1</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>105</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="G23" s="1"/>
       <c r="H23" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
@@ -1482,23 +1482,23 @@
         <v>1</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>106</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="G24" s="1"/>
       <c r="H24" s="2" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
@@ -1540,7 +1540,7 @@
     <hyperlink ref="H5" r:id="rId11"/>
     <hyperlink ref="H13" r:id="rId12"/>
     <hyperlink ref="H21" r:id="rId13"/>
-    <hyperlink ref="H23" r:id="rId14"/>
+    <hyperlink ref="H24" r:id="rId14"/>
     <hyperlink ref="H15" r:id="rId15"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
changed LED's colors, updated BOM and PDF schematic
</commit_message>
<xml_diff>
--- a/H1AR20/Released/BOM/H1AR20.xlsx
+++ b/H1AR20/Released/BOM/H1AR20.xlsx
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="128">
   <si>
     <t>Qty</t>
   </si>
@@ -184,19 +184,10 @@
     <t>https://octopart.com/mmz1608y300b-tdk-368280?r=sp&amp;s=cd9_2ZEqQ9q9UNBuQgHAiA</t>
   </si>
   <si>
-    <t>VLMS1300-GS08</t>
-  </si>
-  <si>
     <t>D1</t>
   </si>
   <si>
-    <t>Red 0603 130ｰ Clear 54 mcd 2 V Surface Mount ChipLED ;</t>
-  </si>
-  <si>
     <t>Vishay</t>
-  </si>
-  <si>
-    <t>https://octopart.com/vlms1300-gs08-vishay-21709201?r=sp&amp;s=_gcP4_q8T1SC6PJQPTQ9yA</t>
   </si>
   <si>
     <t>XTALL_CSTCE8M00G52</t>
@@ -252,21 +243,6 @@
     <t>D2</t>
   </si>
   <si>
-    <t>Cree, Inc.</t>
-  </si>
-  <si>
-    <t>CLVBA-FKA-CC1F1L1BB7R3R3</t>
-  </si>
-  <si>
-    <t>https://octopart.com/clvba-fka-cc1f1l1bb7r3r3-cree-20054005</t>
-  </si>
-  <si>
-    <t>CREE   CLVBA-FKA-CC1F1L1BB7R3R3   LED, HB, RGB, SMD, 130mW</t>
-  </si>
-  <si>
-    <t>Cree CLVBA-FKA-CC1F1L1BB7R3R3</t>
-  </si>
-  <si>
     <t>100nF</t>
   </si>
   <si>
@@ -475,6 +451,24 @@
   </si>
   <si>
     <t>USB-B</t>
+  </si>
+  <si>
+    <t>https://octopart.com/vlmy1300-gs08-vishay-21709204?r=sp</t>
+  </si>
+  <si>
+    <t>VLMY1300-GS08</t>
+  </si>
+  <si>
+    <t>LED Uni-Color Yellow 588nm 2-Pin Chip 0603(1608Metric) T/R</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VLMO1300-GS08 </t>
+  </si>
+  <si>
+    <t>https://octopart.com/vlmo1300-gs08-vishay-21709200?r=sp#</t>
+  </si>
+  <si>
+    <t>LED Uni-Color Soft Orange 611nm 2-Pin Chip 0603(1608Metric) T/R</t>
   </si>
 </sst>
 </file>
@@ -878,7 +872,7 @@
   <dimension ref="A1:I25"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -899,10 +893,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>1</v>
@@ -914,7 +908,7 @@
         <v>3</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="H1" s="3" t="s">
         <v>4</v>
@@ -928,10 +922,10 @@
         <v>8</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>19</v>
@@ -943,7 +937,7 @@
         <v>21</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>24</v>
@@ -960,7 +954,7 @@
         <v>15</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>11</v>
@@ -983,10 +977,10 @@
         <v>29</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>30</v>
@@ -1009,22 +1003,22 @@
         <v>29</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -1035,7 +1029,7 @@
         <v>22</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>19</v>
@@ -1058,25 +1052,25 @@
         <v>1</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -1084,25 +1078,25 @@
         <v>1</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -1110,25 +1104,25 @@
         <v>2</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="E9" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="H9" s="2" t="s">
         <v>65</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -1136,23 +1130,23 @@
         <v>1</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="D10" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="E10" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D10" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>41</v>
-      </c>
       <c r="F10" s="1" t="s">
-        <v>38</v>
+        <v>123</v>
       </c>
       <c r="G10" s="1"/>
       <c r="H10" s="2" t="s">
-        <v>42</v>
+        <v>122</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -1160,23 +1154,23 @@
         <v>1</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>59</v>
+        <v>125</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>58</v>
+        <v>127</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>55</v>
+        <v>39</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>56</v>
+        <v>125</v>
       </c>
       <c r="G11" s="1"/>
       <c r="H11" s="2" t="s">
-        <v>57</v>
+        <v>126</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -1187,7 +1181,7 @@
         <v>33</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>34</v>
@@ -1208,23 +1202,23 @@
         <v>1</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="G13" s="1"/>
       <c r="H13" s="2" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -1232,21 +1226,21 @@
         <v>1</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="E14" s="1"/>
       <c r="F14" s="1" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="G14" s="1"/>
       <c r="H14" s="2" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -1260,7 +1254,7 @@
         <v>26</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>11</v>
@@ -1283,22 +1277,22 @@
         <v>25</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -1309,7 +1303,7 @@
         <v>9</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>10</v>
@@ -1333,22 +1327,22 @@
         <v>18</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -1356,25 +1350,25 @@
         <v>1</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="G19" s="4">
         <v>0.01</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -1382,25 +1376,25 @@
         <v>2</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="G20" s="4">
         <v>0.01</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
@@ -1408,25 +1402,25 @@
         <v>1</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="G21" s="4">
         <v>0.05</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
@@ -1440,7 +1434,7 @@
         <v>6</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>7</v>
@@ -1458,23 +1452,23 @@
         <v>1</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="G23" s="1"/>
       <c r="H23" s="2" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
@@ -1482,23 +1476,23 @@
         <v>1</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="G24" s="1"/>
       <c r="H24" s="2" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
@@ -1506,23 +1500,23 @@
         <v>1</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>30</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="G25" s="1"/>
       <c r="H25" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -1542,8 +1536,9 @@
     <hyperlink ref="H21" r:id="rId13"/>
     <hyperlink ref="H24" r:id="rId14"/>
     <hyperlink ref="H15" r:id="rId15"/>
+    <hyperlink ref="H11" r:id="rId16"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId16"/>
+  <pageSetup orientation="portrait" r:id="rId17"/>
 </worksheet>
 </file>
</xml_diff>